<commit_message>
Allows update of fossil and CO2 emissions from new fuel markets.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-vanadium-redox-flow-battery.xlsx
+++ b/premise/data/additional_inventories/lci-vanadium-redox-flow-battery.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A09718-8D11-2149-8435-BD6A06CCD6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586B25B5-C45E-964C-9CDB-5799B32235D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{26241F67-8618-094B-AD38-E491C9570B84}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$444</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="0.01" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1C5B3A-29A3-3D4D-87B5-E2283E6AD55F}">
   <dimension ref="A1:P444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="B430" sqref="B430"/>
+    <sheetView tabSelected="1" topLeftCell="A420" workbookViewId="0">
+      <selection activeCell="A427" sqref="A427:XFD445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>